<commit_message>
Ajuste de recursos en escaleta Mat 6 tema 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado06\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="1170"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="162">
   <si>
     <t>Asignatura</t>
   </si>
@@ -696,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -850,6 +855,39 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -870,30 +908,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,7 +1181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1178,11 +1192,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="22" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="22" customWidth="1"/>
@@ -1197,7 +1211,7 @@
     <col min="11" max="11" width="16.5703125" style="22" customWidth="1"/>
     <col min="12" max="12" width="20.85546875" style="22" customWidth="1"/>
     <col min="13" max="14" width="8.85546875" style="22" customWidth="1"/>
-    <col min="15" max="15" width="78.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="44.42578125" style="22" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" style="22" customWidth="1"/>
     <col min="17" max="18" width="14.42578125" style="33" customWidth="1"/>
     <col min="19" max="19" width="34" style="51" customWidth="1"/>
@@ -1208,99 +1222,99 @@
     <col min="24" max="16384" width="10.85546875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="59" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="S1" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="T1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="56" t="s">
+      <c r="U1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="57"/>
-    </row>
-    <row r="2" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="62"/>
+      <c r="W1" s="68"/>
+    </row>
+    <row r="2" spans="1:23" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="58"/>
       <c r="M2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="56"/>
-      <c r="W2" s="57"/>
-    </row>
-    <row r="3" spans="1:23" s="14" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+      <c r="W2" s="68"/>
+    </row>
+    <row r="3" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1370,7 @@
       </c>
       <c r="W3" s="15"/>
     </row>
-    <row r="4" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1426,7 @@
       </c>
       <c r="W4" s="15"/>
     </row>
-    <row r="5" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1468,7 +1482,7 @@
       </c>
       <c r="W5" s="15"/>
     </row>
-    <row r="6" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1526,7 +1540,7 @@
       </c>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:23" s="20" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="20" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1581,7 +1595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="20" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="20" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1636,11 +1650,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="20" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="16"/>
+    <row r="9" spans="1:23" s="20" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="E9" s="27" t="s">
         <v>39</v>
       </c>
@@ -1685,7 +1707,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1741,7 +1763,7 @@
       </c>
       <c r="W10" s="15"/>
     </row>
-    <row r="11" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1797,7 +1819,7 @@
       </c>
       <c r="W11" s="15"/>
     </row>
-    <row r="12" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1853,7 +1875,7 @@
       </c>
       <c r="W12" s="15"/>
     </row>
-    <row r="13" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1907,7 +1929,7 @@
       </c>
       <c r="W13" s="15"/>
     </row>
-    <row r="14" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1963,7 +1985,7 @@
       </c>
       <c r="W14" s="15"/>
     </row>
-    <row r="15" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -2019,7 +2041,7 @@
       </c>
       <c r="W15" s="15"/>
     </row>
-    <row r="16" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2075,7 +2097,7 @@
       </c>
       <c r="W16" s="15"/>
     </row>
-    <row r="17" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -2185,7 +2207,7 @@
       </c>
       <c r="W18" s="15"/>
     </row>
-    <row r="19" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -2243,7 +2265,7 @@
       </c>
       <c r="W19" s="15"/>
     </row>
-    <row r="20" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2301,7 +2323,7 @@
       </c>
       <c r="W20" s="15"/>
     </row>
-    <row r="21" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -2359,7 +2381,7 @@
       </c>
       <c r="W21" s="15"/>
     </row>
-    <row r="22" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2415,7 +2437,7 @@
       </c>
       <c r="W22" s="15"/>
     </row>
-    <row r="23" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2471,7 +2493,7 @@
       </c>
       <c r="W23" s="15"/>
     </row>
-    <row r="24" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2529,7 +2551,7 @@
       </c>
       <c r="W24" s="15"/>
     </row>
-    <row r="25" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2585,7 +2607,7 @@
       </c>
       <c r="W25" s="15"/>
     </row>
-    <row r="26" spans="1:23" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="20" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2644,7 +2666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2700,7 +2722,7 @@
       </c>
       <c r="W27" s="15"/>
     </row>
-    <row r="28" spans="1:23" s="20" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" s="20" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +2781,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2819,7 +2841,7 @@
       </c>
       <c r="W29" s="15"/>
     </row>
-    <row r="30" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -2875,7 +2897,7 @@
       </c>
       <c r="W30" s="15"/>
     </row>
-    <row r="31" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -2933,7 +2955,7 @@
       </c>
       <c r="W31" s="15"/>
     </row>
-    <row r="32" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2991,7 +3013,7 @@
       </c>
       <c r="W32" s="15"/>
     </row>
-    <row r="33" spans="1:23" s="14" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -3051,7 +3073,7 @@
       </c>
       <c r="W33" s="15"/>
     </row>
-    <row r="34" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -3109,7 +3131,7 @@
       </c>
       <c r="W34" s="15"/>
     </row>
-    <row r="35" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
@@ -3165,7 +3187,7 @@
       </c>
       <c r="W35" s="15"/>
     </row>
-    <row r="36" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -3209,7 +3231,7 @@
       <c r="U36" s="36"/>
       <c r="W36" s="15"/>
     </row>
-    <row r="37" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
@@ -3267,7 +3289,7 @@
       </c>
       <c r="W37" s="15"/>
     </row>
-    <row r="38" spans="1:23" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -3613,7 +3635,7 @@
       <c r="U50" s="36"/>
       <c r="W50" s="15"/>
     </row>
-    <row r="51" spans="1:23" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" s="14" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="G51" s="21"/>
       <c r="J51" s="21"/>
       <c r="K51" s="22"/>
@@ -3624,7 +3646,7 @@
       <c r="U51" s="23"/>
       <c r="W51" s="23"/>
     </row>
-    <row r="52" spans="1:23" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" s="14" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="G52" s="21"/>
       <c r="J52" s="21"/>
       <c r="K52" s="22"/>
@@ -3645,6 +3667,15 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="21">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3657,15 +3688,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W6 W27 W29:W50 W10:W25">

</xml_diff>

<commit_message>
Mapa conceptual tema 08
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="160">
   <si>
     <t>Asignatura</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Refuerza tu aprendizaje: Las unidades de volumen</t>
   </si>
   <si>
-    <t>Convierte unidades de capacidad y voumen</t>
-  </si>
-  <si>
     <t>Opera con medidas de capacidad y volumen</t>
   </si>
   <si>
@@ -340,9 +337,6 @@
     <t>Refuerza tu aprendizaje: Las unidades de tiempo</t>
   </si>
   <si>
-    <t>Competencias: el conocimiento de las undades de medida</t>
-  </si>
-  <si>
     <t>El proceso de la medición</t>
   </si>
   <si>
@@ -509,13 +503,16 @@
   </si>
   <si>
     <t>Ejercicios de operaciones con medidas de longitud</t>
+  </si>
+  <si>
+    <t>Competencias: el conocimiento de las unidades de medida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,6 +569,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -693,8 +706,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -859,6 +880,30 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -880,32 +925,16 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1176,7 +1205,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1188,7 +1217,7 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -1218,96 +1247,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="60"/>
+      <c r="W1" s="68"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="65"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="58"/>
       <c r="M2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="59"/>
-      <c r="W2" s="60"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+      <c r="W2" s="68"/>
     </row>
     <row r="3" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1320,7 +1349,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="13"/>
@@ -1361,7 +1390,7 @@
         <v>62</v>
       </c>
       <c r="U3" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W3" s="15"/>
     </row>
@@ -1376,7 +1405,7 @@
         <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
@@ -1417,7 +1446,7 @@
         <v>64</v>
       </c>
       <c r="U4" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W4" s="15"/>
     </row>
@@ -1432,7 +1461,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="7"/>
@@ -1488,7 +1517,7 @@
         <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>39</v>
@@ -1504,7 +1533,7 @@
         <v>31</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>24</v>
@@ -1560,7 +1589,7 @@
         <v>33</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>24</v>
@@ -1615,7 +1644,7 @@
         <v>31</v>
       </c>
       <c r="J8" s="42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>24</v>
@@ -1663,7 +1692,7 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H9" s="13">
         <v>7</v>
@@ -1672,7 +1701,7 @@
         <v>31</v>
       </c>
       <c r="J9" s="42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>42</v>
@@ -1713,7 +1742,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="7"/>
@@ -1754,7 +1783,7 @@
         <v>66</v>
       </c>
       <c r="U10" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W10" s="15"/>
     </row>
@@ -1769,7 +1798,7 @@
         <v>61</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="7"/>
@@ -1783,7 +1812,7 @@
         <v>31</v>
       </c>
       <c r="J11" s="40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>24</v>
@@ -1807,7 +1836,7 @@
         <v>35</v>
       </c>
       <c r="T11" s="46" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U11" s="38" t="s">
         <v>36</v>
@@ -1825,7 +1854,7 @@
         <v>61</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="7"/>
@@ -1863,10 +1892,10 @@
         <v>61</v>
       </c>
       <c r="T12" s="45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="U12" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W12" s="15"/>
     </row>
@@ -1881,7 +1910,7 @@
         <v>61</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="7"/>
@@ -1895,7 +1924,7 @@
         <v>23</v>
       </c>
       <c r="J13" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>42</v>
@@ -1917,10 +1946,10 @@
         <v>61</v>
       </c>
       <c r="T13" s="45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U13" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W13" s="15"/>
     </row>
@@ -1935,7 +1964,7 @@
         <v>61</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="7"/>
@@ -1949,7 +1978,7 @@
         <v>31</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>24</v>
@@ -1973,7 +2002,7 @@
         <v>35</v>
       </c>
       <c r="T14" s="46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U14" s="38" t="s">
         <v>36</v>
@@ -1991,14 +2020,14 @@
         <v>61</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H15" s="13">
         <v>13</v>
@@ -2029,10 +2058,10 @@
         <v>61</v>
       </c>
       <c r="T15" s="45" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U15" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W15" s="15"/>
     </row>
@@ -2047,7 +2076,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="7"/>
@@ -2088,7 +2117,7 @@
         <v>78</v>
       </c>
       <c r="U16" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W16" s="15"/>
     </row>
@@ -2103,12 +2132,12 @@
         <v>61</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="7"/>
       <c r="G17" s="41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2141,10 +2170,10 @@
         <v>61</v>
       </c>
       <c r="T17" s="45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U17" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W17" s="15"/>
     </row>
@@ -2159,12 +2188,12 @@
         <v>61</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="7"/>
       <c r="G18" s="41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H18" s="13">
         <v>16</v>
@@ -2195,10 +2224,10 @@
         <v>61</v>
       </c>
       <c r="T18" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U18" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W18" s="15"/>
     </row>
@@ -2213,7 +2242,7 @@
         <v>61</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>39</v>
@@ -2229,7 +2258,7 @@
         <v>31</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>42</v>
@@ -2253,10 +2282,10 @@
         <v>61</v>
       </c>
       <c r="T19" s="45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="U19" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W19" s="15"/>
     </row>
@@ -2271,7 +2300,7 @@
         <v>61</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="7"/>
@@ -2285,7 +2314,7 @@
         <v>31</v>
       </c>
       <c r="J20" s="40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>24</v>
@@ -2329,7 +2358,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" s="27" t="s">
         <v>39</v>
@@ -2345,7 +2374,7 @@
         <v>31</v>
       </c>
       <c r="J21" s="40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>42</v>
@@ -2369,10 +2398,10 @@
         <v>61</v>
       </c>
       <c r="T21" s="45" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U21" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W21" s="15"/>
     </row>
@@ -2387,12 +2416,12 @@
         <v>61</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="7"/>
       <c r="G22" s="40" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="H22" s="13">
         <v>20</v>
@@ -2401,7 +2430,7 @@
         <v>31</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>42</v>
@@ -2425,10 +2454,10 @@
         <v>61</v>
       </c>
       <c r="T22" s="45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="U22" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W22" s="15"/>
     </row>
@@ -2443,12 +2472,12 @@
         <v>61</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="7"/>
       <c r="G23" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -2457,7 +2486,7 @@
         <v>31</v>
       </c>
       <c r="J23" s="40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>42</v>
@@ -2481,10 +2510,10 @@
         <v>61</v>
       </c>
       <c r="T23" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U23" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W23" s="15"/>
     </row>
@@ -2499,14 +2528,14 @@
         <v>61</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E24" s="27" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H24" s="13">
         <v>22</v>
@@ -2515,7 +2544,7 @@
         <v>31</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>42</v>
@@ -2539,10 +2568,10 @@
         <v>61</v>
       </c>
       <c r="T24" s="45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="U24" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W24" s="15"/>
     </row>
@@ -2557,12 +2586,12 @@
         <v>61</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="7"/>
       <c r="G25" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H25" s="13">
         <v>23</v>
@@ -2571,7 +2600,7 @@
         <v>31</v>
       </c>
       <c r="J25" s="40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>42</v>
@@ -2595,10 +2624,10 @@
         <v>61</v>
       </c>
       <c r="T25" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U25" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W25" s="15"/>
     </row>
@@ -2613,12 +2642,12 @@
         <v>61</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="32"/>
       <c r="G26" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H26" s="13">
         <v>24</v>
@@ -2627,7 +2656,7 @@
         <v>31</v>
       </c>
       <c r="J26" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>24</v>
@@ -2640,7 +2669,7 @@
         <v>50</v>
       </c>
       <c r="O26" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P26" s="19" t="s">
         <v>33</v>
@@ -2672,12 +2701,12 @@
         <v>61</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="7"/>
       <c r="G27" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H27" s="13">
         <v>25</v>
@@ -2686,7 +2715,7 @@
         <v>31</v>
       </c>
       <c r="J27" s="40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>42</v>
@@ -2710,10 +2739,10 @@
         <v>61</v>
       </c>
       <c r="T27" s="45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U27" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W27" s="15"/>
     </row>
@@ -2728,12 +2757,12 @@
         <v>61</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="32"/>
       <c r="G28" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H28" s="13">
         <v>26</v>
@@ -2742,7 +2771,7 @@
         <v>33</v>
       </c>
       <c r="J28" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>24</v>
@@ -2755,7 +2784,7 @@
       </c>
       <c r="N28" s="5"/>
       <c r="O28" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P28" s="19" t="s">
         <v>24</v>
@@ -2770,7 +2799,7 @@
         <v>28</v>
       </c>
       <c r="T28" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U28" s="38" t="s">
         <v>30</v>
@@ -2787,12 +2816,12 @@
         <v>61</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="7"/>
       <c r="G29" s="40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -2801,7 +2830,7 @@
         <v>31</v>
       </c>
       <c r="J29" s="40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>24</v>
@@ -2814,7 +2843,7 @@
         <v>50</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P29" s="7" t="s">
         <v>24</v>
@@ -2847,12 +2876,12 @@
         <v>61</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="7"/>
       <c r="G30" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -2861,7 +2890,7 @@
         <v>31</v>
       </c>
       <c r="J30" s="40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>42</v>
@@ -2885,10 +2914,10 @@
         <v>61</v>
       </c>
       <c r="T30" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U30" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W30" s="15"/>
     </row>
@@ -2903,14 +2932,14 @@
         <v>61</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>39</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -2919,7 +2948,7 @@
         <v>31</v>
       </c>
       <c r="J31" s="40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>42</v>
@@ -2943,10 +2972,10 @@
         <v>61</v>
       </c>
       <c r="T31" s="45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="U31" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W31" s="15"/>
     </row>
@@ -2961,12 +2990,12 @@
         <v>61</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="7"/>
       <c r="G32" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H32" s="13">
         <v>30</v>
@@ -2975,7 +3004,7 @@
         <v>23</v>
       </c>
       <c r="J32" s="40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K32" s="6" t="s">
         <v>24</v>
@@ -3001,7 +3030,7 @@
         <v>28</v>
       </c>
       <c r="T32" s="46" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="U32" s="38" t="s">
         <v>30</v>
@@ -3019,12 +3048,12 @@
         <v>61</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="7"/>
       <c r="G33" s="40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" s="13">
         <v>31</v>
@@ -3033,7 +3062,7 @@
         <v>31</v>
       </c>
       <c r="J33" s="40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>24</v>
@@ -3046,7 +3075,7 @@
         <v>44</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P33" s="7" t="s">
         <v>24</v>
@@ -3079,14 +3108,14 @@
         <v>61</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H34" s="13">
         <v>32</v>
@@ -3095,7 +3124,7 @@
         <v>31</v>
       </c>
       <c r="J34" s="40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>42</v>
@@ -3119,10 +3148,10 @@
         <v>61</v>
       </c>
       <c r="T34" s="45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="U34" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W34" s="15"/>
     </row>
@@ -3137,12 +3166,12 @@
         <v>61</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="7"/>
       <c r="G35" s="40" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="H35" s="13">
         <v>33</v>
@@ -3151,7 +3180,7 @@
         <v>31</v>
       </c>
       <c r="J35" s="40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>42</v>
@@ -3175,10 +3204,10 @@
         <v>61</v>
       </c>
       <c r="T35" s="45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U35" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W35" s="15"/>
     </row>
@@ -3207,7 +3236,7 @@
         <v>31</v>
       </c>
       <c r="J36" s="40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K36" s="6" t="s">
         <v>42</v>
@@ -3251,7 +3280,7 @@
         <v>31</v>
       </c>
       <c r="J37" s="40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>24</v>
@@ -3277,7 +3306,7 @@
         <v>35</v>
       </c>
       <c r="T37" s="46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U37" s="38" t="s">
         <v>36</v>
@@ -3309,7 +3338,7 @@
         <v>31</v>
       </c>
       <c r="J38" s="40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>24</v>
@@ -3335,7 +3364,7 @@
         <v>35</v>
       </c>
       <c r="T38" s="46" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="U38" s="38" t="s">
         <v>36</v>
@@ -3662,6 +3691,15 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="21">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3674,15 +3712,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W6 W27 W29:W50 W10:W25">
@@ -3714,6 +3743,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Ajuste de escaleta tema 13
Ajuste de escaleta tema 13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion13/ESCALETA_MA_06_13_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="161">
   <si>
     <t>Asignatura</t>
   </si>
@@ -515,9 +515,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -696,107 +703,107 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -805,105 +812,106 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1187,8 +1195,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
@@ -1218,96 +1226,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="L1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="62" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="60"/>
+      <c r="W1" s="68"/>
     </row>
     <row r="2" spans="1:23" s="14" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="65"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="58"/>
       <c r="M2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="59"/>
-      <c r="W2" s="60"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+      <c r="W2" s="68"/>
     </row>
     <row r="3" spans="1:23" s="14" customFormat="1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1573,7 +1581,9 @@
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="18"/>
+      <c r="P7" s="73" t="s">
+        <v>24</v>
+      </c>
       <c r="Q7" s="38">
         <v>6</v>
       </c>
@@ -1796,7 +1806,9 @@
         <v>59</v>
       </c>
       <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="P11" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="Q11" s="38">
         <v>6</v>
       </c>
@@ -1962,7 +1974,9 @@
         <v>37</v>
       </c>
       <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="P14" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="Q14" s="38">
         <v>6</v>
       </c>
@@ -2698,7 +2712,7 @@
       <c r="N27" s="5"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Q27" s="38">
         <v>7</v>
@@ -3662,6 +3676,15 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="21">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3674,15 +3697,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W6 W27 W29:W50 W10:W25">

</xml_diff>